<commit_message>
Some corrections have been made
</commit_message>
<xml_diff>
--- a/PowerQuery/Original Data/Import_Folder/Import_W1.xlsx
+++ b/PowerQuery/Original Data/Import_Folder/Import_W1.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\Documents\GitHub_Excel\PowerQuery\Original Data\Import_Folder\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E090B295-3A4C-4891-B57F-12254A7B2B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -321,15 +331,17 @@
     <t>94368</t>
   </si>
   <si>
-    <t xml:space="preserve">data generated with OnlineDataGenerator available at: https://www.onlinedatagenerator.com </t>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>W1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -347,11 +359,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3D3D3" tint="0"/>
+        <fgColor rgb="FFD3D3D3"/>
       </patternFill>
     </fill>
   </fills>
@@ -368,35 +380,340 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.43" customWidth="1"/>
-    <col min="2" max="2" width="14.43" customWidth="1"/>
-    <col min="3" max="3" width="14.9792262486049" customWidth="1"/>
-    <col min="4" max="4" width="20.8655722481864" customWidth="1"/>
-    <col min="5" max="5" width="14.43" customWidth="1"/>
+    <col min="1" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,353 +729,411 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+      <c r="F1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+      <c r="F5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
+      <c r="F8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
+      <c r="F10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
+      <c r="F12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
+      <c r="F13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
+      <c r="F14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
+      <c r="F15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
+      <c r="F16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
+      <c r="F18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0" t="s">
+      <c r="F19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="0" t="s">
+      <c r="F20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="0" t="s">
-        <v>103</v>
+      <c r="F21" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>